<commit_message>
Ditto - New exel
</commit_message>
<xml_diff>
--- a/SSAS/Development/Artifacts/Changes From 13 April.xlsx
+++ b/SSAS/Development/Artifacts/Changes From 13 April.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -39,6 +39,9 @@
   <si>
     <t>Comments (What was changed and need to be tested)</t>
   </si>
+  <si>
+    <t>How is done by Developer (Explain in detail)</t>
+  </si>
 </sst>
 </file>
 
@@ -61,15 +64,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,25 +86,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,376 +425,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="72.42578125" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="39.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="60.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="2"/>
+      <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="C42" s="1"/>
+      <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="C43" s="1"/>
+      <c r="G43" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D45" s="2"/>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="2"/>
+      <c r="C46" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -778,10 +808,61 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -790,7 +871,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
@@ -809,7 +890,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003520CC91E1C90A4F9689A135D663C63F" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bea9beecb72e899f05172e22af69af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e967487d-3eea-483d-b969-e50e6c114ffa" xmlns:ns3="43475cab-d89f-451e-a1e3-4db005e0f558" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="438d5435a0413bb8242127eebe6f163c" ns2:_="" ns3:_="">
     <xsd:import namespace="e967487d-3eea-483d-b969-e50e6c114ffa"/>
@@ -993,57 +1074,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1051,7 +1090,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1068,7 +1107,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0051AA5-43D6-41A0-9086-D5D3DFF72221}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1085,12 +1124,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ditto Pachen- Merge from Branch April 29
</commit_message>
<xml_diff>
--- a/SSAS/Development/Artifacts/Changes From 13 April.xlsx
+++ b/SSAS/Development/Artifacts/Changes From 13 April.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -41,6 +41,121 @@
   </si>
   <si>
     <t>How is done by Developer (Explain in detail)</t>
+  </si>
+  <si>
+    <t>New Files
+EJBServer\components\MOLSA\message\MOLSABpoNumberToArabic.xml
+EJBServer\components\MOLSA\source\curam\molsa\util\impl\MOLSANumberToArabic.java
+Changed Files
+EJBServer\components\MOLSA\message\MOLSABpoGenerateEFT.xml
+EJBServer\components\MOLSA\source\curam\molsa\util\impl\MOLSAGenerateEFTHelper.java
+EJBServer\components\MOLSA\source\curam\molsa\eft\batch\impl\MOLSAGenerateEFTBatchStream.java
+EJBServer\components\MOLSA\properties\Application.prx
+model/Packages/EFT/Batch.efx</t>
+  </si>
+  <si>
+    <t>EFT Generation</t>
+  </si>
+  <si>
+    <t>Ditto</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Only the Application.prx change (use insertproperties and change back the production details)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use build insertProperties and change back the production varaiables.                                                                                                         UPDATE PROPERTIES SET VALUE='غانم  مبارك الكواري' WHERE NAME='curam.molsa.financial.eft.nameOfAssistanceMinisterForSocialAffair';
+UPDATE PROPERTIES SET VALUE='احمد نصر النصر' WHERE NAME='curam.molsa.financial.eft.nameOfSocialSecurityDirector';
+UPDATE PROPERTIES SET VALUE='مدير الضمان الاجتماعي' WHERE NAME='curam.molsa.financial.eft.mswordSignatureTitleOne'
+UPDATE PROPERTIES SET VALUE='وكيل الوزارة المشاعد للشؤون الاجتماعية' WHERE NAME='curam.molsa.financial.eft.mswordSignatureTitleTwo';
+New Values  (Use admin screen to add these values)
+curam.molsa.financial.eft.currencyCode
+curam.molsa.financial.eft.companyAccountNumber
+curam.molsa.financial.eft.dateFormat
+curam.molsa.financial.eft.ministryLetterAddressLine1
+curam.molsa.financial.eft.printAmountInWords
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EJBServer\components\MOLSA_ar\tab\FamilyOfPrisoner\FamilyOfPrisonerProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\MaidAssistance\MaidAssistanceProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\DivorcedLady\DivorcedLadyProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Widow\WidowProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\FamilyOfMissing\FamilyOfMissingPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\ExceptionCase\ExceptionCaseProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\DesertedWife\DesertedWifeProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\FamilyInNeed\FamilyInNeedPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\IncapableOfWorking\IncapableOfWorkingPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\AnonymousParents\AnonymousParentsPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\SeniorCitizen\SeniorCitizenPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\FamilyOfMissing\FamilyOfMissingProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Handicap\HandicapPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Orphan\OrphanPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\FamilyOfPrisoner\FamilyOfPrisonerPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\MaidAssistance\MaidAssistancePDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\DivorcedLady\DivorcedLadyPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Widow\WidowPDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\FamilyInNeed\FamilyInNeedProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\ExceptionCase\ExceptionCasePDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\DesertedWife\DesertedWifePDProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\IncapableOfWorking\IncapableOfWorkingProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\AnonymousParents\AnonymousParentsProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\SeniorCitizen\SeniorCitizenProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Handicap\HandicapProductDisplay_ar.properties  
+EJBServer\components\MOLSA_ar\tab\Orphan\OrphanProductDisplay_ar.properties  
+</t>
+  </si>
+  <si>
+    <t>Smitha</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EJBServer\components\MOLSA\data\initial\blob\MOLSASMSMessageText.properties
+EJBServer\components\MOLSA_ar\data\initial\blob\MOLSASMSMessageTextArabic.properties
+</t>
+  </si>
+  <si>
+    <t>Properties were changed in English and Arabic</t>
+  </si>
+  <si>
+    <t>Upload the changed properties through  admin</t>
+  </si>
+  <si>
+    <t>Added new files for the Arabic translations
+upload the new properties</t>
+  </si>
+  <si>
+    <t>New entries were added to 
+EJBServer\components\MOLSA\data\initial\rules\CREOLEPRODUCTDECISIONDISPCAT.dmx
+EJBServer\components\MOLSA\data\initial\rules\CREOLEPRODUCTPERIODDISPCAT.dmx
+EJBServer\components\MOLSA\data\initial\rules\CREOLERULECLASSLINK.dmx
+EJBServer\components\MOLSA\CREOLE_Rule_Sets\ExceptionCaseDisplayRuleSet.xml
+New file added is
+EJBServer\components\MOLSA\CREOLE_Rule_Sets\SocialAssistance\ExceptionCase\ExceptionCaseUnitInformation.xml</t>
+  </si>
+  <si>
+    <t>Use build and upload ruleset to upload the ruleset
+Execute the mentioned SQL queries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+INSERT INTO CREOLEPRODUCTPERIODDISPCAT (CREOLEPRODUCTPERIODDISPCATID, CREOLEPRODUCTPERIODID, CREOLEPRODUCTDECISIONDISPCATID, DECISIONDETAILSRCLID, VERSIONNO) VALUES (4550, 4512, 4550, 4605, 1);
+INSERT INTO CREOLEPRODUCTDECISIONDISPCAT (CREOLEPRODUCTDECISIONDISPCATID, PRODUCTID, NAMEID, DISPLAYORDER, DISPLAYPAGENAME, CATEGORYREF, VERSIONNO) VALUES (4550, 45012, 4563, 3, 'None', 'unitInformation', 1);
+INSERT INTO CREOLERULECLASSLINK (CREOLERULECLASSLINKID, CREOLERULESETID, RULECLASSNAME, VERSIONNO) VALUES (4605, 4549, 'ExceptionCaseUnitInformation', 1);
+</t>
+  </si>
+  <si>
+    <t>EJBServer\components\MOLSA\source\curam\molsa\core\sl\impl\MOLSAEvidenceControllerInterfaceImpl.java</t>
+  </si>
+  <si>
+    <t>Added conditions</t>
+  </si>
+  <si>
+    <t>Changed the Class file.</t>
   </si>
 </sst>
 </file>
@@ -110,9 +225,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -121,6 +233,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,385 +540,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="72.42578125" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="39.140625" customWidth="1"/>
     <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="60.28515625" customWidth="1"/>
+    <col min="9" max="9" width="53.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+    <row r="2" spans="1:9" ht="375" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>42120</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+    <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>42122</v>
+      </c>
+      <c r="B3">
+        <v>372</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>42122</v>
+      </c>
+      <c r="B4">
+        <v>371</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+    <row r="5" spans="1:9" ht="360" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>42117</v>
+      </c>
+      <c r="B5">
+        <v>375</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="1"/>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>42118</v>
+      </c>
+      <c r="B6">
+        <v>376</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E40 C37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
       <formula1>"Swathi,Sneha,Ashwal,Rajesh,Harisha,Deepu,Ditto,Ramesh,Smitha"</formula1>
     </dataValidation>
   </dataValidations>
@@ -813,6 +711,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
+      <Description>UQKZYU5EZKJQ-17-950</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -860,34 +786,6 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
-      <Description>UQKZYU5EZKJQ-17-950</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1075,22 +973,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1103,6 +985,22 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>